<commit_message>
added needed caps, fixed a spelling error
</commit_message>
<xml_diff>
--- a/connectors.xlsx
+++ b/connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Altium-Lib-Tom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrne\Altium-Lib-Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183B4030-C984-4EFA-8FC3-D62234FF84DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA875D-CC78-4F41-B46F-82C907FB6764}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9338" activeTab="2" xr2:uid="{78D20A57-1DED-49B5-B563-D879E43957A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9345" xr2:uid="{78D20A57-1DED-49B5-B563-D879E43957A9}"/>
   </bookViews>
   <sheets>
     <sheet name="audio" sheetId="1" r:id="rId1"/>
@@ -460,19 +460,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2836C16-527F-40CD-92B2-0E8CE5C6790A}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="4"/>
-    <col min="6" max="6" width="9.06640625" style="4"/>
+    <col min="3" max="3" width="9" style="4"/>
+    <col min="6" max="6" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,11 +525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" t="str">
-        <f>"RES-"&amp;TEXT(ROW()-1,"000000")</f>
-        <v>RES-000001</v>
-      </c>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>1</v>
       </c>
@@ -562,9 +558,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6D77F4-42AE-41B8-94B0-862C2658C3CC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -574,9 +572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0BB6F6-1A63-43C6-BD30-76210C90D84C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new db sheets, new connector symbols
</commit_message>
<xml_diff>
--- a/connectors.xlsx
+++ b/connectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrne\Altium-Lib-Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA875D-CC78-4F41-B46F-82C907FB6764}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70803FC-4EEC-4B92-A011-4364F01C3B2C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9345" xr2:uid="{78D20A57-1DED-49B5-B563-D879E43957A9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>TPN</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Through-Hole</t>
   </si>
   <si>
-    <t>RES</t>
-  </si>
-  <si>
     <t>Footprint Ref</t>
   </si>
   <si>
-    <t>RES-TH</t>
-  </si>
-  <si>
     <t>Manufacturer 1</t>
   </si>
   <si>
@@ -95,6 +89,30 @@
   </si>
   <si>
     <t>Library Ref</t>
+  </si>
+  <si>
+    <t>STEREO_JACK</t>
+  </si>
+  <si>
+    <t>MONO_JACK</t>
+  </si>
+  <si>
+    <t>STEREO_JACK_HDR</t>
+  </si>
+  <si>
+    <t>MONO_JACK_HDR</t>
+  </si>
+  <si>
+    <t>PWR_JACK_HDR</t>
+  </si>
+  <si>
+    <t>PWR_JACK_SW_HDR</t>
+  </si>
+  <si>
+    <t>9V_BATT</t>
+  </si>
+  <si>
+    <t>PWR_JACK_SW</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2836C16-527F-40CD-92B2-0E8CE5C6790A}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +488,8 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="4"/>
     <col min="6" max="6" width="9" style="4"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -495,16 +515,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -513,16 +533,16 @@
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -542,10 +562,18 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -556,26 +584,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6D77F4-42AE-41B8-94B0-862C2658C3CC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0BB6F6-1A63-43C6-BD30-76210C90D84C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated jacks and switches
</commit_message>
<xml_diff>
--- a/connectors.xlsx
+++ b/connectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrne\Altium-Lib-Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70803FC-4EEC-4B92-A011-4364F01C3B2C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD09FC30-7664-47B0-B39F-013326F5328D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9345" xr2:uid="{78D20A57-1DED-49B5-B563-D879E43957A9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="127">
   <si>
     <t>TPN</t>
   </si>
@@ -40,33 +40,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Tolerance</t>
-  </si>
-  <si>
-    <t>Power Rating</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Pulse-Rated</t>
-  </si>
-  <si>
     <t>Supplier 1</t>
   </si>
   <si>
     <t>Supplier 1 PN</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Through-Hole</t>
-  </si>
-  <si>
     <t>Footprint Ref</t>
   </si>
   <si>
@@ -113,13 +92,334 @@
   </si>
   <si>
     <t>PWR_JACK_SW</t>
+  </si>
+  <si>
+    <t>BATTERY CONNECT SNAP 9V 4" LEADS</t>
+  </si>
+  <si>
+    <t>Battery Type Function</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Battery Cell Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Cells </t>
+  </si>
+  <si>
+    <t>Battery Series</t>
+  </si>
+  <si>
+    <t>Mounting Type</t>
+  </si>
+  <si>
+    <t>Termination Style</t>
+  </si>
+  <si>
+    <t>Height Above Board</t>
+  </si>
+  <si>
+    <t>Operating Temperature</t>
+  </si>
+  <si>
+    <t>Connector, Snap</t>
+  </si>
+  <si>
+    <t>9V</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Free Hanging</t>
+  </si>
+  <si>
+    <t>Wire Leads - 4" (101.6mm)</t>
+  </si>
+  <si>
+    <t>Supplier 1 Link</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>36-232-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/keystone-electronics/232/36-232-ND/303804</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 2X5.5MM SOLDER</t>
+  </si>
+  <si>
+    <t>CUI Inc.</t>
+  </si>
+  <si>
+    <t>Connector Type</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Industry Recognized Mating Diamter</t>
+  </si>
+  <si>
+    <t>Actual Diameter</t>
+  </si>
+  <si>
+    <t>Number of Positions/Contacts</t>
+  </si>
+  <si>
+    <t>PJ-011A</t>
+  </si>
+  <si>
+    <t>CP-011A-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cui-inc/PJ-011A/CP-011A-ND/305540</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2.10mm ID (0.083"), 5.50mm OD (0.217")</t>
+  </si>
+  <si>
+    <t>0.079" (2.00mm ID), 0.236" (6.00mm OD)</t>
+  </si>
+  <si>
+    <t>2 Conductors, 3 Contacts</t>
+  </si>
+  <si>
+    <t>Internal Switch(s)</t>
+  </si>
+  <si>
+    <t>Mounting Feature</t>
+  </si>
+  <si>
+    <t>Termination</t>
+  </si>
+  <si>
+    <t>Shielding</t>
+  </si>
+  <si>
+    <t>Single Switch, Normally Closed</t>
+  </si>
+  <si>
+    <t>Panel Mount</t>
+  </si>
+  <si>
+    <t>Bulkhead - Front Side Nut</t>
+  </si>
+  <si>
+    <t>Solder Eyelet(s)</t>
+  </si>
+  <si>
+    <t>Unshielded</t>
+  </si>
+  <si>
+    <t>Mounting Hardware, Thread Lock</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Insulation Color</t>
+  </si>
+  <si>
+    <t>Voltage - Rated</t>
+  </si>
+  <si>
+    <t>Current Rating</t>
+  </si>
+  <si>
+    <t>12VDC</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>Mating Length / Depth</t>
+  </si>
+  <si>
+    <t>Ingress Protection</t>
+  </si>
+  <si>
+    <t>Contact Material - Plating</t>
+  </si>
+  <si>
+    <t>Body Material</t>
+  </si>
+  <si>
+    <t>Includes</t>
+  </si>
+  <si>
+    <t>Housing Material</t>
+  </si>
+  <si>
+    <t>Contact Material</t>
+  </si>
+  <si>
+    <t>Thread Size</t>
+  </si>
+  <si>
+    <t>Body Color</t>
+  </si>
+  <si>
+    <t>Material Flammability Rating</t>
+  </si>
+  <si>
+    <t>Nickel</t>
+  </si>
+  <si>
+    <t>2 pcs - 1 Connector, 1 Nut</t>
+  </si>
+  <si>
+    <t>Polyoxymethylene (POM)</t>
+  </si>
+  <si>
+    <t>Brass; Copper Alloy</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>UL94 V-0</t>
+  </si>
+  <si>
+    <t>CONN JACK STEREO 6.35MM PNL MNT</t>
+  </si>
+  <si>
+    <t>Supplier 2 Link</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/switchcraft-inc/12B/SC1094-ND/109541</t>
+  </si>
+  <si>
+    <t>SC1094-ND</t>
+  </si>
+  <si>
+    <t>Switchcraft Inc</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>Singal Lines</t>
+  </si>
+  <si>
+    <t>Industry Recognized Mating Diameter</t>
+  </si>
+  <si>
+    <t>mating Length/Depth</t>
+  </si>
+  <si>
+    <t>Cable Opening</t>
+  </si>
+  <si>
+    <t>Panel Hole Size</t>
+  </si>
+  <si>
+    <t>LITTLE-JAX</t>
+  </si>
+  <si>
+    <t>Phone Jack</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Stereo (3 Conductor, TRS)</t>
+  </si>
+  <si>
+    <t>6.35mm (0.250", 1/4") - Headphone</t>
+  </si>
+  <si>
+    <t>0.25" (6.35mm)</t>
+  </si>
+  <si>
+    <t>3 Conductors, 3 Contacts</t>
+  </si>
+  <si>
+    <t>Does Not Contain Switch</t>
+  </si>
+  <si>
+    <t>Panel Mount, Through Hole</t>
+  </si>
+  <si>
+    <t>25VDC</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>Copper Alloy</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>3 pcs - 1 Connector, 1 Nut, 1 Washer</t>
+  </si>
+  <si>
+    <t>0.375" (9.52mm)</t>
+  </si>
+  <si>
+    <t>3/8"-32</t>
+  </si>
+  <si>
+    <t>-20°C ~ 65°C</t>
+  </si>
+  <si>
+    <t>Mammoth Electronics</t>
+  </si>
+  <si>
+    <t>JK100S</t>
+  </si>
+  <si>
+    <t>https://www.mammothelectronics.com/collections/audio-jacks/products/4sjk100s</t>
+  </si>
+  <si>
+    <t>JK100M</t>
+  </si>
+  <si>
+    <t>https://www.mammothelectronics.com/collections/audio-jacks/products/4sjk100m</t>
+  </si>
+  <si>
+    <t>FAL11</t>
+  </si>
+  <si>
+    <t>SC1847-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/switchcraft-inc/FAL11/SC1847-ND/1289066</t>
+  </si>
+  <si>
+    <t>CONN JACK MONO 6.35MM PNL MNT</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>2 Conductors, 2 Contacts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +434,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,12 +462,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2836C16-527F-40CD-92B2-0E8CE5C6790A}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,11 +796,11 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="4"/>
     <col min="6" max="6" width="9" style="4"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.7109375" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,80 +808,352 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"AUD-CN-"&amp;TEXT(ROW()-1,"0000")</f>
+        <v>AUD-CN-0001</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" t="s">
+        <v>111</v>
+      </c>
+      <c r="V2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AD2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>"AUD-CN-"&amp;TEXT(ROW()-1,"0000")</f>
+        <v>AUD-CN-0002</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" t="s">
+        <v>110</v>
+      </c>
+      <c r="U3" t="s">
+        <v>111</v>
+      </c>
+      <c r="V3" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="AD3" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="E2">
-        <v>0.125</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
+      <c r="AE3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -584,15 +1164,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6D77F4-42AE-41B8-94B0-862C2658C3CC}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="27" width="37.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,57 +1187,217 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"PWR-CN-"&amp;TEXT(ROW()-1,"0000")</f>
+        <v>PWR-CN-0001</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
+      <c r="AD2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -660,15 +1407,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0BB6F6-1A63-43C6-BD30-76210C90D84C}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,60 +1428,125 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"BATT-"&amp;TEXT(ROW()-1,"0000")</f>
+        <v>BATT-0001</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2">
+        <v>232</v>
+      </c>
+      <c r="P2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>